<commit_message>
adding dummy command to CMOS to access first ring buffer element
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836CF34F-B828-DE45-83EB-7325D135D6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E1207D-2AF9-8845-BC83-D4186759E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="207">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -354,9 +354,6 @@
     <t>0x7d</t>
   </si>
   <si>
-    <t>0x38000248</t>
-  </si>
-  <si>
     <t>noop</t>
   </si>
   <si>
@@ -555,9 +552,6 @@
     <t>0x0000021c</t>
   </si>
   <si>
-    <t>0x38000240</t>
-  </si>
-  <si>
     <t>read_ring_ql_rd_ptr</t>
   </si>
   <si>
@@ -567,9 +561,6 @@
     <t>read_ring_wr_ptr</t>
   </si>
   <si>
-    <t>0x38000220</t>
-  </si>
-  <si>
     <t>rd_ptr</t>
   </si>
   <si>
@@ -643,6 +634,27 @@
   </si>
   <si>
     <t>read CMOS data file write pointer</t>
+  </si>
+  <si>
+    <t>read_ring_start</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>0x00000240</t>
+  </si>
+  <si>
+    <t>0x00000248</t>
+  </si>
+  <si>
+    <t>0x00000220</t>
+  </si>
+  <si>
+    <t>0x00001000</t>
+  </si>
+  <si>
+    <t>0x1e0000</t>
   </si>
 </sst>
 </file>
@@ -1142,13 +1154,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC57"/>
+  <dimension ref="A1:AC58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC29" sqref="AC29"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1316,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E28" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E29" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1605,7 +1617,7 @@
         <v>61</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -1650,7 +1662,7 @@
         <v>104</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA6" s="25" t="s">
         <v>57</v>
@@ -1664,7 +1676,7 @@
     </row>
     <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>72</v>
@@ -1692,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K7" s="23" t="s">
         <v>102</v>
@@ -1740,7 +1752,7 @@
         <v>104</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>57</v>
@@ -1749,12 +1761,12 @@
         <v>100</v>
       </c>
       <c r="AC7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>72</v>
@@ -1782,7 +1794,7 @@
         <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K8" s="23" t="s">
         <v>102</v>
@@ -1830,7 +1842,7 @@
         <v>104</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA8" s="25" t="s">
         <v>57</v>
@@ -1839,12 +1851,12 @@
         <v>100</v>
       </c>
       <c r="AC8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>72</v>
@@ -1872,7 +1884,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K9" s="23" t="s">
         <v>102</v>
@@ -1920,7 +1932,7 @@
         <v>104</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AA9" s="25" t="s">
         <v>57</v>
@@ -1929,12 +1941,12 @@
         <v>100</v>
       </c>
       <c r="AC9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>72</v>
@@ -1962,7 +1974,7 @@
         <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>102</v>
@@ -2010,7 +2022,7 @@
         <v>104</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>57</v>
@@ -2019,7 +2031,7 @@
         <v>100</v>
       </c>
       <c r="AC10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2100,7 +2112,7 @@
         <v>104</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA11" s="25" t="s">
         <v>57</v>
@@ -2109,12 +2121,12 @@
         <v>100</v>
       </c>
       <c r="AC11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>72</v>
@@ -2190,7 +2202,7 @@
         <v>104</v>
       </c>
       <c r="Z12" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA12" s="25" t="s">
         <v>57</v>
@@ -2199,7 +2211,7 @@
         <v>100</v>
       </c>
       <c r="AC12" s="28" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2232,7 +2244,7 @@
         <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>102</v>
@@ -2280,7 +2292,7 @@
         <v>104</v>
       </c>
       <c r="Z13" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA13" s="25" t="s">
         <v>57</v>
@@ -2289,12 +2301,12 @@
         <v>100</v>
       </c>
       <c r="AC13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>72</v>
@@ -2322,7 +2334,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>102</v>
@@ -2370,7 +2382,7 @@
         <v>104</v>
       </c>
       <c r="Z14" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AA14" s="25" t="s">
         <v>57</v>
@@ -2379,12 +2391,12 @@
         <v>100</v>
       </c>
       <c r="AC14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>72</v>
@@ -2412,7 +2424,7 @@
         <v>17</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K15" s="23" t="s">
         <v>102</v>
@@ -2460,7 +2472,7 @@
         <v>104</v>
       </c>
       <c r="Z15" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>57</v>
@@ -2469,12 +2481,12 @@
         <v>100</v>
       </c>
       <c r="AC15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>72</v>
@@ -2550,7 +2562,7 @@
         <v>104</v>
       </c>
       <c r="Z16" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA16" s="25" t="s">
         <v>57</v>
@@ -2559,12 +2571,12 @@
         <v>100</v>
       </c>
       <c r="AC16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>72</v>
@@ -2640,7 +2652,7 @@
         <v>104</v>
       </c>
       <c r="Z17" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA17" s="25" t="s">
         <v>57</v>
@@ -2649,12 +2661,12 @@
         <v>100</v>
       </c>
       <c r="AC17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>72</v>
@@ -2730,7 +2742,7 @@
         <v>104</v>
       </c>
       <c r="Z18" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AA18" s="25" t="s">
         <v>57</v>
@@ -2739,12 +2751,12 @@
         <v>100</v>
       </c>
       <c r="AC18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>72</v>
@@ -2820,7 +2832,7 @@
         <v>104</v>
       </c>
       <c r="Z19" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AA19" s="25" t="s">
         <v>57</v>
@@ -2829,12 +2841,12 @@
         <v>100</v>
       </c>
       <c r="AC19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>72</v>
@@ -2910,7 +2922,7 @@
         <v>104</v>
       </c>
       <c r="Z20" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AA20" s="25" t="s">
         <v>57</v>
@@ -2919,12 +2931,12 @@
         <v>100</v>
       </c>
       <c r="AC20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>72</v>
@@ -2952,7 +2964,7 @@
         <v>17</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K21" s="23" t="s">
         <v>102</v>
@@ -3000,7 +3012,7 @@
         <v>104</v>
       </c>
       <c r="Z21" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA21" s="25" t="s">
         <v>57</v>
@@ -3009,12 +3021,12 @@
         <v>100</v>
       </c>
       <c r="AC21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>72</v>
@@ -3042,7 +3054,7 @@
         <v>17</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K22" s="23" t="s">
         <v>102</v>
@@ -3090,7 +3102,7 @@
         <v>104</v>
       </c>
       <c r="Z22" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AA22" s="25" t="s">
         <v>57</v>
@@ -3099,12 +3111,12 @@
         <v>100</v>
       </c>
       <c r="AC22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>72</v>
@@ -3132,7 +3144,7 @@
         <v>17</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>102</v>
@@ -3180,7 +3192,7 @@
         <v>104</v>
       </c>
       <c r="Z23" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AA23" s="25" t="s">
         <v>57</v>
@@ -3189,12 +3201,12 @@
         <v>100</v>
       </c>
       <c r="AC23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>72</v>
@@ -3222,7 +3234,7 @@
         <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K24" s="23" t="s">
         <v>102</v>
@@ -3270,7 +3282,7 @@
         <v>104</v>
       </c>
       <c r="Z24" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AA24" s="25" t="s">
         <v>57</v>
@@ -3279,12 +3291,12 @@
         <v>100</v>
       </c>
       <c r="AC24" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>72</v>
@@ -3312,7 +3324,7 @@
         <v>17</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K25" s="23" t="s">
         <v>102</v>
@@ -3360,7 +3372,7 @@
         <v>104</v>
       </c>
       <c r="Z25" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AA25" s="25" t="s">
         <v>57</v>
@@ -3369,12 +3381,12 @@
         <v>100</v>
       </c>
       <c r="AC25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>72</v>
@@ -3402,7 +3414,7 @@
         <v>17</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K26" s="23" t="s">
         <v>102</v>
@@ -3450,7 +3462,7 @@
         <v>104</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="AA26" s="25" t="s">
         <v>57</v>
@@ -3459,12 +3471,12 @@
         <v>100</v>
       </c>
       <c r="AC26" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>72</v>
@@ -3492,7 +3504,7 @@
         <v>17</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K27" s="23" t="s">
         <v>102</v>
@@ -3540,7 +3552,7 @@
         <v>104</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="AA27" s="23" t="s">
         <v>57</v>
@@ -3549,12 +3561,12 @@
         <v>100</v>
       </c>
       <c r="AC27" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>72</v>
@@ -3630,7 +3642,7 @@
         <v>104</v>
       </c>
       <c r="Z28" s="27" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="AA28" s="25" t="s">
         <v>57</v>
@@ -3639,130 +3651,130 @@
         <v>100</v>
       </c>
       <c r="AC28" s="28" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="17"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="24"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="24"/>
+    <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="27">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10">
+        <v>10101</v>
+      </c>
+      <c r="E29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0x95</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L29" s="30">
+        <v>0</v>
+      </c>
+      <c r="M29" s="30">
+        <v>0</v>
+      </c>
+      <c r="N29" s="30">
+        <v>0</v>
+      </c>
+      <c r="O29" s="30">
+        <v>0</v>
+      </c>
+      <c r="P29" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="30">
+        <v>0</v>
+      </c>
+      <c r="R29" s="30">
+        <v>0</v>
+      </c>
+      <c r="S29" s="30">
+        <v>0</v>
+      </c>
+      <c r="T29" s="30">
+        <v>0</v>
+      </c>
+      <c r="U29" s="30">
+        <v>1</v>
+      </c>
+      <c r="V29" s="30">
+        <v>1</v>
+      </c>
+      <c r="W29" s="31">
+        <v>0</v>
+      </c>
+      <c r="X29" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y29" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z29" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA29" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB29" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC29" s="28" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="10">
-        <v>1000000</v>
-      </c>
-      <c r="E30" s="3" t="str">
-        <f t="shared" ref="E30:E55" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C30,7) + BIN2DEC($D30)))</f>
-        <v>0x40</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L30" s="6">
-        <v>0</v>
-      </c>
-      <c r="M30" s="6">
-        <v>1</v>
-      </c>
-      <c r="N30" s="6">
-        <v>0</v>
-      </c>
-      <c r="O30" s="6">
-        <v>0</v>
-      </c>
-      <c r="P30" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>0</v>
-      </c>
-      <c r="R30" s="6">
-        <v>0</v>
-      </c>
-      <c r="S30" s="6">
-        <v>0</v>
-      </c>
-      <c r="T30" s="6">
-        <v>0</v>
-      </c>
-      <c r="U30" s="6">
-        <v>0</v>
-      </c>
-      <c r="V30" s="6">
-        <v>0</v>
-      </c>
-      <c r="W30" s="16">
-        <v>0</v>
-      </c>
-      <c r="X30" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y30" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA30" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>77</v>
-      </c>
+    <row r="30" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="24"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="24"/>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>72</v>
@@ -3771,11 +3783,11 @@
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>1000010</v>
+        <v>1000000</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x42</v>
+        <f t="shared" ref="E31:E56" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C31,7) + BIN2DEC($D31)))</f>
+        <v>0x40</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>53</v>
@@ -3847,12 +3859,12 @@
         <v>100</v>
       </c>
       <c r="AC31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>72</v>
@@ -3861,17 +3873,17 @@
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>1000100</v>
+        <v>1000010</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x44</v>
+        <v>0x42</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>17</v>
@@ -3886,10 +3898,10 @@
         <v>57</v>
       </c>
       <c r="L32" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32" s="6">
         <v>0</v>
@@ -3937,12 +3949,12 @@
         <v>100</v>
       </c>
       <c r="AC32" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>72</v>
@@ -3951,11 +3963,11 @@
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>1000101</v>
+        <v>1000100</v>
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x45</v>
+        <v>0x44</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>17</v>
@@ -4032,7 +4044,7 @@
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>72</v>
@@ -4041,17 +4053,17 @@
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>1110111</v>
+        <v>1000101</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0x45</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>17</v>
@@ -4117,12 +4129,12 @@
         <v>100</v>
       </c>
       <c r="AC34" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>72</v>
@@ -4131,14 +4143,14 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>1100001</v>
+        <v>1110111</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x77</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35">
         <v>2</v>
@@ -4156,7 +4168,7 @@
         <v>57</v>
       </c>
       <c r="L35" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="6">
         <v>0</v>
@@ -4168,19 +4180,19 @@
         <v>0</v>
       </c>
       <c r="P35" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R35" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T35" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U35" s="6">
         <v>0</v>
@@ -4189,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="W35" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X35" s="13" t="s">
         <v>97</v>
@@ -4207,12 +4219,12 @@
         <v>100</v>
       </c>
       <c r="AC35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>72</v>
@@ -4221,17 +4233,17 @@
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>1100010</v>
+        <v>1100001</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x61</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>17</v>
@@ -4297,12 +4309,12 @@
         <v>100</v>
       </c>
       <c r="AC36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>72</v>
@@ -4311,11 +4323,11 @@
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>1100011</v>
+        <v>1100010</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x62</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>17</v>
@@ -4387,12 +4399,12 @@
         <v>100</v>
       </c>
       <c r="AC37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>72</v>
@@ -4401,11 +4413,11 @@
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>100100</v>
+        <v>1100011</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x24</v>
+        <v>0x63</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>17</v>
@@ -4426,10 +4438,10 @@
         <v>57</v>
       </c>
       <c r="L38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" s="6">
         <v>0</v>
@@ -4453,10 +4465,10 @@
         <v>1</v>
       </c>
       <c r="U38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W38" s="16">
         <v>1</v>
@@ -4477,12 +4489,12 @@
         <v>100</v>
       </c>
       <c r="AC38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>72</v>
@@ -4491,11 +4503,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>100101</v>
+        <v>100100</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x25</v>
+        <v>0x24</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>17</v>
@@ -4567,12 +4579,12 @@
         <v>100</v>
       </c>
       <c r="AC39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
-        <v>108</v>
+    <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>72</v>
@@ -4581,11 +4593,11 @@
         <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>11000</v>
+        <v>100101</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C40,7) + BIN2DEC($D40)))</f>
-        <v>0x18</v>
+        <f t="shared" si="1"/>
+        <v>0x25</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>17</v>
@@ -4606,10 +4618,10 @@
         <v>57</v>
       </c>
       <c r="L40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" s="6">
         <v>0</v>
@@ -4618,19 +4630,19 @@
         <v>0</v>
       </c>
       <c r="P40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40" s="6">
         <v>1</v>
@@ -4639,7 +4651,7 @@
         <v>1</v>
       </c>
       <c r="W40" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X40" s="13" t="s">
         <v>97</v>
@@ -4648,21 +4660,21 @@
         <v>105</v>
       </c>
       <c r="Z40" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA40" s="23" t="s">
-        <v>146</v>
+        <v>57</v>
+      </c>
+      <c r="AA40" s="23">
+        <v>0</v>
       </c>
       <c r="AB40" t="s">
         <v>100</v>
       </c>
       <c r="AC40" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>72</v>
@@ -4671,11 +4683,11 @@
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>11111</v>
+        <v>11000</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1F</v>
+        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C41,7) + BIN2DEC($D41)))</f>
+        <v>0x18</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -4689,7 +4701,7 @@
       <c r="I41" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K41" s="23" t="s">
@@ -4738,21 +4750,21 @@
         <v>105</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AA41" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB41" t="s">
         <v>100</v>
       </c>
       <c r="AC41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>72</v>
@@ -4761,11 +4773,11 @@
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>10000</v>
+        <v>11111</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x10</v>
+        <v>0x1F</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>17</v>
@@ -4828,21 +4840,21 @@
         <v>105</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AA42" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB42" t="s">
         <v>100</v>
       </c>
       <c r="AC42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>107</v>
+      <c r="A43" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>72</v>
@@ -4851,11 +4863,11 @@
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>10001</v>
+        <v>10000</v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x11</v>
+        <v>0x10</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>17</v>
@@ -4918,21 +4930,21 @@
         <v>105</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="AA43" s="23" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="AB43" t="s">
         <v>100</v>
       </c>
       <c r="AC43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
-        <v>118</v>
+      <c r="A44" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>72</v>
@@ -4941,11 +4953,11 @@
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>10010</v>
+        <v>10001</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x12</v>
+        <v>0x11</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>17</v>
@@ -5008,21 +5020,21 @@
         <v>105</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="AA44" s="23" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="AB44" t="s">
         <v>100</v>
       </c>
       <c r="AC44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>72</v>
@@ -5031,11 +5043,11 @@
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x13</v>
+        <v>0x12</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>17</v>
@@ -5098,21 +5110,21 @@
         <v>105</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AA45" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB45" t="s">
         <v>100</v>
       </c>
       <c r="AC45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>50</v>
+      <c r="A46" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>72</v>
@@ -5121,17 +5133,17 @@
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>11010</v>
+        <v>10011</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1A</v>
+        <v>0x13</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>17</v>
@@ -5139,7 +5151,7 @@
       <c r="I46" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="3" t="s">
+      <c r="J46" t="s">
         <v>17</v>
       </c>
       <c r="K46" s="23" t="s">
@@ -5158,25 +5170,25 @@
         <v>0</v>
       </c>
       <c r="P46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U46" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V46" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W46" s="16">
         <v>0</v>
@@ -5188,21 +5200,21 @@
         <v>105</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA46" s="23">
-        <v>0</v>
+        <v>123</v>
+      </c>
+      <c r="AA46" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="AB46" t="s">
         <v>100</v>
       </c>
       <c r="AC46" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>72</v>
@@ -5211,17 +5223,17 @@
         <v>0</v>
       </c>
       <c r="D47" s="10">
-        <v>11100</v>
+        <v>11010</v>
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1C</v>
+        <v>0x1A</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G47" t="s">
-        <v>97</v>
+        <v>51</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>17</v>
@@ -5287,12 +5299,12 @@
         <v>100</v>
       </c>
       <c r="AC47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>72</v>
@@ -5301,14 +5313,14 @@
         <v>0</v>
       </c>
       <c r="D48" s="10">
-        <v>11101</v>
+        <v>11100</v>
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1D</v>
+        <v>0x1C</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="G48" t="s">
         <v>97</v>
@@ -5377,12 +5389,12 @@
         <v>100</v>
       </c>
       <c r="AC48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>72</v>
@@ -5391,14 +5403,14 @@
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>111010</v>
+        <v>11101</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3A</v>
+        <v>0x1D</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="G49" t="s">
         <v>97</v>
@@ -5428,25 +5440,25 @@
         <v>0</v>
       </c>
       <c r="P49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W49" s="16">
         <v>0</v>
@@ -5467,12 +5479,12 @@
         <v>100</v>
       </c>
       <c r="AC49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>72</v>
@@ -5481,11 +5493,11 @@
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <v>111011</v>
+        <v>111010</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3B</v>
+        <v>0x3A</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>99</v>
@@ -5557,12 +5569,12 @@
         <v>100</v>
       </c>
       <c r="AC50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>72</v>
@@ -5571,17 +5583,17 @@
         <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>111001</v>
+        <v>111011</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x39</v>
+        <v>0x3B</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="G51" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>17</v>
@@ -5596,7 +5608,7 @@
         <v>57</v>
       </c>
       <c r="L51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51" s="6">
         <v>0</v>
@@ -5623,10 +5635,10 @@
         <v>0</v>
       </c>
       <c r="U51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W51" s="16">
         <v>0</v>
@@ -5647,12 +5659,12 @@
         <v>100</v>
       </c>
       <c r="AC51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
-        <v>36</v>
+      <c r="A52" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>72</v>
@@ -5661,11 +5673,11 @@
         <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>1110000</v>
+        <v>111001</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x39</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>17</v>
@@ -5686,7 +5698,7 @@
         <v>57</v>
       </c>
       <c r="L52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" s="6">
         <v>0</v>
@@ -5713,12 +5725,12 @@
         <v>0</v>
       </c>
       <c r="U52" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V52" s="6">
-        <v>1</v>
-      </c>
-      <c r="W52" s="6">
+        <v>0</v>
+      </c>
+      <c r="W52" s="16">
         <v>0</v>
       </c>
       <c r="X52" s="13" t="s">
@@ -5728,21 +5740,21 @@
         <v>105</v>
       </c>
       <c r="Z52" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA52" s="23" t="s">
-        <v>146</v>
+        <v>57</v>
+      </c>
+      <c r="AA52" s="23">
+        <v>0</v>
       </c>
       <c r="AB52" t="s">
         <v>100</v>
       </c>
       <c r="AC52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>72</v>
@@ -5751,11 +5763,11 @@
         <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>1110001</v>
+        <v>1110000</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x70</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>17</v>
@@ -5821,18 +5833,18 @@
         <v>151</v>
       </c>
       <c r="AA53" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB53" t="s">
         <v>100</v>
       </c>
       <c r="AC53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>72</v>
@@ -5841,11 +5853,11 @@
         <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>1110010</v>
+        <v>1110001</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x71</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>17</v>
@@ -5911,18 +5923,18 @@
         <v>150</v>
       </c>
       <c r="AA54" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB54" t="s">
         <v>100</v>
       </c>
       <c r="AC54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>72</v>
@@ -5931,11 +5943,11 @@
         <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>1110011</v>
+        <v>1110010</v>
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x72</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>17</v>
@@ -6001,18 +6013,18 @@
         <v>149</v>
       </c>
       <c r="AA55" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB55" t="s">
         <v>100</v>
       </c>
       <c r="AC55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>72</v>
@@ -6021,11 +6033,11 @@
         <v>0</v>
       </c>
       <c r="D56" s="10">
-        <v>1110100</v>
+        <v>1110011</v>
       </c>
       <c r="E56" s="3" t="str">
-        <f t="shared" ref="E56:E57" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C56,7) + BIN2DEC($D56)))</f>
-        <v>0x74</v>
+        <f t="shared" si="1"/>
+        <v>0x73</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>17</v>
@@ -6091,18 +6103,18 @@
         <v>148</v>
       </c>
       <c r="AA56" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AB56" t="s">
         <v>100</v>
       </c>
       <c r="AC56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>72</v>
@@ -6111,82 +6123,172 @@
         <v>0</v>
       </c>
       <c r="D57" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E57" s="3" t="str">
+        <f t="shared" ref="E57:E58" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C57,7) + BIN2DEC($D57)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L57" s="6">
+        <v>0</v>
+      </c>
+      <c r="M57" s="6">
+        <v>0</v>
+      </c>
+      <c r="N57" s="6">
+        <v>0</v>
+      </c>
+      <c r="O57" s="6">
+        <v>0</v>
+      </c>
+      <c r="P57" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>0</v>
+      </c>
+      <c r="R57" s="6">
+        <v>0</v>
+      </c>
+      <c r="S57" s="6">
+        <v>0</v>
+      </c>
+      <c r="T57" s="6">
+        <v>0</v>
+      </c>
+      <c r="U57" s="6">
+        <v>1</v>
+      </c>
+      <c r="V57" s="6">
+        <v>1</v>
+      </c>
+      <c r="W57" s="6">
+        <v>0</v>
+      </c>
+      <c r="X57" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y57" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z57" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA57" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0</v>
+      </c>
+      <c r="D58" s="10">
         <v>1111000</v>
       </c>
-      <c r="E57" s="3" t="str">
+      <c r="E58" s="3" t="str">
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57" t="s">
-        <v>17</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I57" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K57" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L57" s="6">
-        <v>0</v>
-      </c>
-      <c r="M57" s="6">
-        <v>0</v>
-      </c>
-      <c r="N57" s="6">
-        <v>0</v>
-      </c>
-      <c r="O57" s="6">
-        <v>0</v>
-      </c>
-      <c r="P57" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="6">
-        <v>0</v>
-      </c>
-      <c r="R57" s="6">
-        <v>0</v>
-      </c>
-      <c r="S57" s="6">
-        <v>0</v>
-      </c>
-      <c r="T57" s="6">
-        <v>0</v>
-      </c>
-      <c r="U57" s="6">
-        <v>1</v>
-      </c>
-      <c r="V57" s="6">
-        <v>1</v>
-      </c>
-      <c r="W57" s="6">
-        <v>0</v>
-      </c>
-      <c r="X57" s="13" t="s">
+      <c r="F58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L58" s="6">
+        <v>0</v>
+      </c>
+      <c r="M58" s="6">
+        <v>0</v>
+      </c>
+      <c r="N58" s="6">
+        <v>0</v>
+      </c>
+      <c r="O58" s="6">
+        <v>0</v>
+      </c>
+      <c r="P58" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>0</v>
+      </c>
+      <c r="R58" s="6">
+        <v>0</v>
+      </c>
+      <c r="S58" s="6">
+        <v>0</v>
+      </c>
+      <c r="T58" s="6">
+        <v>0</v>
+      </c>
+      <c r="U58" s="6">
+        <v>1</v>
+      </c>
+      <c r="V58" s="6">
+        <v>1</v>
+      </c>
+      <c r="W58" s="6">
+        <v>0</v>
+      </c>
+      <c r="X58" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y57" s="22" t="s">
+      <c r="Y58" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="Z57" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA57" s="23" t="s">
+      <c r="Z58" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AB57" t="s">
+      <c r="AA58" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB58" t="s">
         <v>100</v>
       </c>
-      <c r="AC57" t="s">
+      <c r="AC58" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying other CMOS buffer read size
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E1207D-2AF9-8845-BC83-D4186759E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC004CA1-FD8C-1F41-8E46-EF55DA575752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -654,7 +654,7 @@
     <t>0x00001000</t>
   </si>
   <si>
-    <t>0x1e0000</t>
+    <t>0x061a80</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
trying Ethernet packet as max CMOS size
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC004CA1-FD8C-1F41-8E46-EF55DA575752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D4C4D6-4171-7B4A-892C-F42D79CF2BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -654,7 +654,7 @@
     <t>0x00001000</t>
   </si>
   <si>
-    <t>0x061a80</t>
+    <t>0x05a0</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
trying to read just above MTU
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D4C4D6-4171-7B4A-892C-F42D79CF2BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40557E2-A518-6F40-8315-BDD5433BAC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -654,7 +654,7 @@
     <t>0x00001000</t>
   </si>
   <si>
-    <t>0x05a0</t>
+    <t>0x060f</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding size of CMOS ring buffer data
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40557E2-A518-6F40-8315-BDD5433BAC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10476DA1-D5DB-5245-889F-B5D69DA9DF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="214">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -655,6 +655,27 @@
   </si>
   <si>
     <t>0x060f</t>
+  </si>
+  <si>
+    <t>read_ring_ql_size</t>
+  </si>
+  <si>
+    <t>rd_size</t>
+  </si>
+  <si>
+    <t>0x00000244</t>
+  </si>
+  <si>
+    <t>0x0000024c</t>
+  </si>
+  <si>
+    <t>read_ring_pc_size</t>
+  </si>
+  <si>
+    <t>read CMOS PC size</t>
+  </si>
+  <si>
+    <t>read CMOS QL size</t>
   </si>
 </sst>
 </file>
@@ -1154,13 +1175,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC58"/>
+  <dimension ref="A1:AC60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomRight" activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1328,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E29" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E31" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -3476,7 +3497,7 @@
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>72</v>
@@ -3485,11 +3506,11 @@
         <v>1</v>
       </c>
       <c r="D27" s="10">
-        <v>10010</v>
+        <v>10001</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x92</v>
+        <v>0x91</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>17</v>
@@ -3504,7 +3525,7 @@
         <v>17</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="K27" s="23" t="s">
         <v>102</v>
@@ -3552,7 +3573,7 @@
         <v>104</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="AA27" s="23" t="s">
         <v>57</v>
@@ -3561,400 +3582,400 @@
         <v>100</v>
       </c>
       <c r="AC27" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" s="26" t="s">
+      <c r="A28" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="10">
-        <v>10100</v>
+        <v>10010</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x94</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="K28" s="25" t="s">
+        <v>0x92</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K28" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="L28" s="30">
-        <v>0</v>
-      </c>
-      <c r="M28" s="30">
-        <v>0</v>
-      </c>
-      <c r="N28" s="30">
-        <v>0</v>
-      </c>
-      <c r="O28" s="30">
-        <v>0</v>
-      </c>
-      <c r="P28" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="30">
-        <v>0</v>
-      </c>
-      <c r="R28" s="30">
-        <v>0</v>
-      </c>
-      <c r="S28" s="30">
-        <v>0</v>
-      </c>
-      <c r="T28" s="30">
-        <v>0</v>
-      </c>
-      <c r="U28" s="30">
-        <v>1</v>
-      </c>
-      <c r="V28" s="30">
-        <v>1</v>
-      </c>
-      <c r="W28" s="31">
-        <v>0</v>
-      </c>
-      <c r="X28" s="29" t="s">
+      <c r="L28" s="6">
+        <v>0</v>
+      </c>
+      <c r="M28" s="6">
+        <v>0</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0</v>
+      </c>
+      <c r="O28" s="6">
+        <v>0</v>
+      </c>
+      <c r="P28" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>0</v>
+      </c>
+      <c r="R28" s="6">
+        <v>0</v>
+      </c>
+      <c r="S28" s="6">
+        <v>0</v>
+      </c>
+      <c r="T28" s="6">
+        <v>0</v>
+      </c>
+      <c r="U28" s="6">
+        <v>1</v>
+      </c>
+      <c r="V28" s="6">
+        <v>1</v>
+      </c>
+      <c r="W28" s="16">
+        <v>0</v>
+      </c>
+      <c r="X28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y28" s="32" t="s">
+      <c r="Y28" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="Z28" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="AA28" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB28" s="28" t="s">
+      <c r="Z28" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA28" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB28" t="s">
         <v>100</v>
       </c>
-      <c r="AC28" s="28" t="s">
-        <v>199</v>
+      <c r="AC28" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" s="10">
-        <v>10101</v>
+        <v>10011</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x95</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="K29" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="L29" s="30">
-        <v>0</v>
-      </c>
-      <c r="M29" s="30">
-        <v>0</v>
-      </c>
-      <c r="N29" s="30">
-        <v>0</v>
-      </c>
-      <c r="O29" s="30">
-        <v>0</v>
-      </c>
-      <c r="P29" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="30">
-        <v>0</v>
-      </c>
-      <c r="R29" s="30">
-        <v>0</v>
-      </c>
-      <c r="S29" s="30">
-        <v>0</v>
-      </c>
-      <c r="T29" s="30">
-        <v>0</v>
-      </c>
-      <c r="U29" s="30">
-        <v>1</v>
-      </c>
-      <c r="V29" s="30">
-        <v>1</v>
-      </c>
-      <c r="W29" s="31">
-        <v>0</v>
-      </c>
-      <c r="X29" s="29" t="s">
+        <v>0x93</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="L29" s="6">
+        <v>0</v>
+      </c>
+      <c r="M29" s="6">
+        <v>0</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0</v>
+      </c>
+      <c r="O29" s="6">
+        <v>0</v>
+      </c>
+      <c r="P29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>0</v>
+      </c>
+      <c r="R29" s="6">
+        <v>0</v>
+      </c>
+      <c r="S29" s="6">
+        <v>0</v>
+      </c>
+      <c r="T29" s="6">
+        <v>0</v>
+      </c>
+      <c r="U29" s="6">
+        <v>1</v>
+      </c>
+      <c r="V29" s="6">
+        <v>1</v>
+      </c>
+      <c r="W29" s="16">
+        <v>0</v>
+      </c>
+      <c r="X29" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y29" s="32" t="s">
+      <c r="Y29" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="Z29" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA29" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB29" s="28" t="s">
+      <c r="Z29" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA29" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB29" t="s">
         <v>100</v>
       </c>
-      <c r="AC29" s="28" t="s">
+      <c r="AC29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="27">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10">
+        <v>10100</v>
+      </c>
+      <c r="E30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0x94</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="L30" s="30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="30">
+        <v>0</v>
+      </c>
+      <c r="N30" s="30">
+        <v>0</v>
+      </c>
+      <c r="O30" s="30">
+        <v>0</v>
+      </c>
+      <c r="P30" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="30">
+        <v>0</v>
+      </c>
+      <c r="R30" s="30">
+        <v>0</v>
+      </c>
+      <c r="S30" s="30">
+        <v>0</v>
+      </c>
+      <c r="T30" s="30">
+        <v>0</v>
+      </c>
+      <c r="U30" s="30">
+        <v>1</v>
+      </c>
+      <c r="V30" s="30">
+        <v>1</v>
+      </c>
+      <c r="W30" s="31">
+        <v>0</v>
+      </c>
+      <c r="X30" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y30" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z30" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA30" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB30" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC30" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="30" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="24"/>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="18" t="s">
+      <c r="A31" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="3">
-        <v>0</v>
+      <c r="C31" s="27">
+        <v>1</v>
       </c>
       <c r="D31" s="10">
-        <v>1000000</v>
+        <v>10101</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f t="shared" ref="E31:E56" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C31,7) + BIN2DEC($D31)))</f>
-        <v>0x40</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L31" s="6">
-        <v>0</v>
-      </c>
-      <c r="M31" s="6">
-        <v>1</v>
-      </c>
-      <c r="N31" s="6">
-        <v>0</v>
-      </c>
-      <c r="O31" s="6">
-        <v>0</v>
-      </c>
-      <c r="P31" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>0</v>
-      </c>
-      <c r="R31" s="6">
-        <v>0</v>
-      </c>
-      <c r="S31" s="6">
-        <v>0</v>
-      </c>
-      <c r="T31" s="6">
-        <v>0</v>
-      </c>
-      <c r="U31" s="6">
-        <v>0</v>
-      </c>
-      <c r="V31" s="6">
-        <v>0</v>
-      </c>
-      <c r="W31" s="16">
-        <v>0</v>
-      </c>
-      <c r="X31" s="13" t="s">
+        <f t="shared" si="0"/>
+        <v>0x95</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L31" s="30">
+        <v>0</v>
+      </c>
+      <c r="M31" s="30">
+        <v>0</v>
+      </c>
+      <c r="N31" s="30">
+        <v>0</v>
+      </c>
+      <c r="O31" s="30">
+        <v>0</v>
+      </c>
+      <c r="P31" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="30">
+        <v>0</v>
+      </c>
+      <c r="R31" s="30">
+        <v>0</v>
+      </c>
+      <c r="S31" s="30">
+        <v>0</v>
+      </c>
+      <c r="T31" s="30">
+        <v>0</v>
+      </c>
+      <c r="U31" s="30">
+        <v>1</v>
+      </c>
+      <c r="V31" s="30">
+        <v>1</v>
+      </c>
+      <c r="W31" s="31">
+        <v>0</v>
+      </c>
+      <c r="X31" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="Y31" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA31" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB31" t="s">
+      <c r="Y31" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z31" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA31" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB31" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="AC31" t="s">
-        <v>77</v>
+      <c r="AC31" s="28" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="10">
-        <v>1000010</v>
-      </c>
-      <c r="E32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x42</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L32" s="6">
-        <v>0</v>
-      </c>
-      <c r="M32" s="6">
-        <v>1</v>
-      </c>
-      <c r="N32" s="6">
-        <v>0</v>
-      </c>
-      <c r="O32" s="6">
-        <v>0</v>
-      </c>
-      <c r="P32" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="6">
-        <v>0</v>
-      </c>
-      <c r="R32" s="6">
-        <v>0</v>
-      </c>
-      <c r="S32" s="6">
-        <v>0</v>
-      </c>
-      <c r="T32" s="6">
-        <v>0</v>
-      </c>
-      <c r="U32" s="6">
-        <v>0</v>
-      </c>
-      <c r="V32" s="6">
-        <v>0</v>
-      </c>
-      <c r="W32" s="16">
-        <v>0</v>
-      </c>
-      <c r="X32" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y32" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA32" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>78</v>
-      </c>
+    <row r="32" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="24"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="24"/>
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>72</v>
@@ -3963,17 +3984,17 @@
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>1000100</v>
+        <v>1000000</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x44</v>
+        <f t="shared" ref="E33:E58" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C33,7) + BIN2DEC($D33)))</f>
+        <v>0x40</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>17</v>
@@ -3988,10 +4009,10 @@
         <v>57</v>
       </c>
       <c r="L33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="6">
         <v>0</v>
@@ -4039,12 +4060,12 @@
         <v>100</v>
       </c>
       <c r="AC33" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>72</v>
@@ -4053,17 +4074,17 @@
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>1000101</v>
+        <v>1000010</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x45</v>
+        <v>0x42</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>17</v>
@@ -4078,10 +4099,10 @@
         <v>57</v>
       </c>
       <c r="L34" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="6">
         <v>0</v>
@@ -4129,12 +4150,12 @@
         <v>100</v>
       </c>
       <c r="AC34" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>72</v>
@@ -4143,17 +4164,17 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>1110111</v>
+        <v>1000100</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0x44</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G35">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>17</v>
@@ -4219,12 +4240,12 @@
         <v>100</v>
       </c>
       <c r="AC35" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>72</v>
@@ -4233,17 +4254,17 @@
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>1100001</v>
+        <v>1000101</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x45</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>17</v>
@@ -4258,7 +4279,7 @@
         <v>57</v>
       </c>
       <c r="L36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="6">
         <v>0</v>
@@ -4270,19 +4291,19 @@
         <v>0</v>
       </c>
       <c r="P36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U36" s="6">
         <v>0</v>
@@ -4291,7 +4312,7 @@
         <v>0</v>
       </c>
       <c r="W36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X36" s="13" t="s">
         <v>97</v>
@@ -4309,12 +4330,12 @@
         <v>100</v>
       </c>
       <c r="AC36" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>72</v>
@@ -4323,17 +4344,17 @@
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>1100010</v>
+        <v>1110111</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x77</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>17</v>
@@ -4348,7 +4369,7 @@
         <v>57</v>
       </c>
       <c r="L37" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="6">
         <v>0</v>
@@ -4360,19 +4381,19 @@
         <v>0</v>
       </c>
       <c r="P37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U37" s="6">
         <v>0</v>
@@ -4381,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="W37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X37" s="13" t="s">
         <v>97</v>
@@ -4399,12 +4420,12 @@
         <v>100</v>
       </c>
       <c r="AC37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>72</v>
@@ -4413,17 +4434,17 @@
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>1100011</v>
+        <v>1100001</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x61</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>17</v>
@@ -4489,12 +4510,12 @@
         <v>100</v>
       </c>
       <c r="AC38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>72</v>
@@ -4503,11 +4524,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>100100</v>
+        <v>1100010</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x24</v>
+        <v>0x62</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>17</v>
@@ -4528,10 +4549,10 @@
         <v>57</v>
       </c>
       <c r="L39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39" s="6">
         <v>0</v>
@@ -4555,10 +4576,10 @@
         <v>1</v>
       </c>
       <c r="U39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W39" s="16">
         <v>1</v>
@@ -4579,12 +4600,12 @@
         <v>100</v>
       </c>
       <c r="AC39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>72</v>
@@ -4593,11 +4614,11 @@
         <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>100101</v>
+        <v>1100011</v>
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x25</v>
+        <v>0x63</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>17</v>
@@ -4618,10 +4639,10 @@
         <v>57</v>
       </c>
       <c r="L40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40" s="6">
         <v>0</v>
@@ -4645,10 +4666,10 @@
         <v>1</v>
       </c>
       <c r="U40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W40" s="16">
         <v>1</v>
@@ -4669,12 +4690,12 @@
         <v>100</v>
       </c>
       <c r="AC40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
-        <v>107</v>
+    <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>72</v>
@@ -4683,11 +4704,11 @@
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>11000</v>
+        <v>100100</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C41,7) + BIN2DEC($D41)))</f>
-        <v>0x18</v>
+        <f t="shared" si="1"/>
+        <v>0x24</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -4708,10 +4729,10 @@
         <v>57</v>
       </c>
       <c r="L41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N41" s="6">
         <v>0</v>
@@ -4720,19 +4741,19 @@
         <v>0</v>
       </c>
       <c r="P41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U41" s="6">
         <v>1</v>
@@ -4741,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="W41" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X41" s="13" t="s">
         <v>97</v>
@@ -4750,21 +4771,21 @@
         <v>105</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA41" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA41" s="23">
+        <v>0</v>
       </c>
       <c r="AB41" t="s">
         <v>100</v>
       </c>
       <c r="AC41" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
-        <v>114</v>
+      <c r="A42" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>72</v>
@@ -4773,11 +4794,11 @@
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>11111</v>
+        <v>100101</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1F</v>
+        <v>0x25</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>17</v>
@@ -4791,17 +4812,17 @@
       <c r="I42" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>57</v>
       </c>
       <c r="L42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N42" s="6">
         <v>0</v>
@@ -4810,19 +4831,19 @@
         <v>0</v>
       </c>
       <c r="P42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T42" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U42" s="6">
         <v>1</v>
@@ -4831,7 +4852,7 @@
         <v>1</v>
       </c>
       <c r="W42" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X42" s="13" t="s">
         <v>97</v>
@@ -4840,21 +4861,21 @@
         <v>105</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA42" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA42" s="23">
+        <v>0</v>
       </c>
       <c r="AB42" t="s">
         <v>100</v>
       </c>
       <c r="AC42" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>72</v>
@@ -4863,11 +4884,11 @@
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10</v>
+        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C43,7) + BIN2DEC($D43)))</f>
+        <v>0x18</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>17</v>
@@ -4881,7 +4902,7 @@
       <c r="I43" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K43" s="23" t="s">
@@ -4930,7 +4951,7 @@
         <v>105</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AA43" s="23" t="s">
         <v>145</v>
@@ -4939,12 +4960,12 @@
         <v>100</v>
       </c>
       <c r="AC43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>106</v>
+      <c r="A44" s="19" t="s">
+        <v>114</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>72</v>
@@ -4953,11 +4974,11 @@
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>10001</v>
+        <v>11111</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x11</v>
+        <v>0x1F</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>17</v>
@@ -5020,21 +5041,21 @@
         <v>105</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="AA44" s="23" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="AB44" t="s">
         <v>100</v>
       </c>
       <c r="AC44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>72</v>
@@ -5043,11 +5064,11 @@
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>10010</v>
+        <v>10000</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x12</v>
+        <v>0x10</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>17</v>
@@ -5110,7 +5131,7 @@
         <v>105</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA45" s="23" t="s">
         <v>145</v>
@@ -5119,12 +5140,12 @@
         <v>100</v>
       </c>
       <c r="AC45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
-        <v>115</v>
+      <c r="A46" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>72</v>
@@ -5133,11 +5154,11 @@
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>10011</v>
+        <v>10001</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x13</v>
+        <v>0x11</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>17</v>
@@ -5200,21 +5221,21 @@
         <v>105</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="AA46" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="AB46" t="s">
         <v>100</v>
       </c>
       <c r="AC46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>50</v>
+      <c r="A47" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>72</v>
@@ -5223,17 +5244,17 @@
         <v>0</v>
       </c>
       <c r="D47" s="10">
-        <v>11010</v>
+        <v>10010</v>
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1A</v>
+        <v>0x12</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G47" t="s">
+        <v>17</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>17</v>
@@ -5241,7 +5262,7 @@
       <c r="I47" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="J47" t="s">
         <v>17</v>
       </c>
       <c r="K47" s="23" t="s">
@@ -5260,25 +5281,25 @@
         <v>0</v>
       </c>
       <c r="P47" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R47" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T47" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U47" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V47" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="16">
         <v>0</v>
@@ -5290,21 +5311,21 @@
         <v>105</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA47" s="23">
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="AA47" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="AB47" t="s">
         <v>100</v>
       </c>
       <c r="AC47" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>47</v>
+      <c r="A48" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>72</v>
@@ -5313,17 +5334,17 @@
         <v>0</v>
       </c>
       <c r="D48" s="10">
-        <v>11100</v>
+        <v>10011</v>
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1C</v>
+        <v>0x13</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="G48" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>17</v>
@@ -5331,7 +5352,7 @@
       <c r="I48" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J48" s="3" t="s">
+      <c r="J48" t="s">
         <v>17</v>
       </c>
       <c r="K48" s="23" t="s">
@@ -5350,25 +5371,25 @@
         <v>0</v>
       </c>
       <c r="P48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W48" s="16">
         <v>0</v>
@@ -5380,21 +5401,21 @@
         <v>105</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA48" s="23">
-        <v>0</v>
+        <v>123</v>
+      </c>
+      <c r="AA48" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="AB48" t="s">
         <v>100</v>
       </c>
       <c r="AC48" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>72</v>
@@ -5403,17 +5424,17 @@
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>11101</v>
+        <v>11010</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1D</v>
+        <v>0x1A</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G49" t="s">
-        <v>97</v>
+        <v>51</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>17</v>
@@ -5479,12 +5500,12 @@
         <v>100</v>
       </c>
       <c r="AC49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>72</v>
@@ -5493,14 +5514,14 @@
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <v>111010</v>
+        <v>11100</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3A</v>
+        <v>0x1C</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G50" t="s">
         <v>97</v>
@@ -5530,25 +5551,25 @@
         <v>0</v>
       </c>
       <c r="P50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W50" s="16">
         <v>0</v>
@@ -5569,12 +5590,12 @@
         <v>100</v>
       </c>
       <c r="AC50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>72</v>
@@ -5583,14 +5604,14 @@
         <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>111011</v>
+        <v>11101</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3B</v>
+        <v>0x1D</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="G51" t="s">
         <v>97</v>
@@ -5620,25 +5641,25 @@
         <v>0</v>
       </c>
       <c r="P51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W51" s="16">
         <v>0</v>
@@ -5659,12 +5680,12 @@
         <v>100</v>
       </c>
       <c r="AC51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>72</v>
@@ -5673,17 +5694,17 @@
         <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>111001</v>
+        <v>111010</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x39</v>
+        <v>0x3A</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="G52" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>17</v>
@@ -5698,7 +5719,7 @@
         <v>57</v>
       </c>
       <c r="L52" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" s="6">
         <v>0</v>
@@ -5725,10 +5746,10 @@
         <v>0</v>
       </c>
       <c r="U52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W52" s="16">
         <v>0</v>
@@ -5749,12 +5770,12 @@
         <v>100</v>
       </c>
       <c r="AC52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="19" t="s">
-        <v>36</v>
+      <c r="A53" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>72</v>
@@ -5763,17 +5784,17 @@
         <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>1110000</v>
+        <v>111011</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x3B</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="G53" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>17</v>
@@ -5820,7 +5841,7 @@
       <c r="V53" s="6">
         <v>1</v>
       </c>
-      <c r="W53" s="6">
+      <c r="W53" s="16">
         <v>0</v>
       </c>
       <c r="X53" s="13" t="s">
@@ -5830,21 +5851,21 @@
         <v>105</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA53" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA53" s="23">
+        <v>0</v>
       </c>
       <c r="AB53" t="s">
         <v>100</v>
       </c>
       <c r="AC53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="19" t="s">
-        <v>37</v>
+      <c r="A54" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>72</v>
@@ -5853,11 +5874,11 @@
         <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>1110001</v>
+        <v>111001</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x39</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>17</v>
@@ -5878,7 +5899,7 @@
         <v>57</v>
       </c>
       <c r="L54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="6">
         <v>0</v>
@@ -5905,12 +5926,12 @@
         <v>0</v>
       </c>
       <c r="U54" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V54" s="6">
-        <v>1</v>
-      </c>
-      <c r="W54" s="6">
+        <v>0</v>
+      </c>
+      <c r="W54" s="16">
         <v>0</v>
       </c>
       <c r="X54" s="13" t="s">
@@ -5920,21 +5941,21 @@
         <v>105</v>
       </c>
       <c r="Z54" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA54" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA54" s="23">
+        <v>0</v>
       </c>
       <c r="AB54" t="s">
         <v>100</v>
       </c>
       <c r="AC54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>72</v>
@@ -5943,11 +5964,11 @@
         <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>1110010</v>
+        <v>1110000</v>
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x70</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>17</v>
@@ -6010,7 +6031,7 @@
         <v>105</v>
       </c>
       <c r="Z55" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AA55" s="23" t="s">
         <v>145</v>
@@ -6019,12 +6040,12 @@
         <v>100</v>
       </c>
       <c r="AC55" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>72</v>
@@ -6033,11 +6054,11 @@
         <v>0</v>
       </c>
       <c r="D56" s="10">
-        <v>1110011</v>
+        <v>1110001</v>
       </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x71</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>17</v>
@@ -6100,7 +6121,7 @@
         <v>105</v>
       </c>
       <c r="Z56" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AA56" s="23" t="s">
         <v>145</v>
@@ -6109,12 +6130,12 @@
         <v>100</v>
       </c>
       <c r="AC56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>72</v>
@@ -6123,11 +6144,11 @@
         <v>0</v>
       </c>
       <c r="D57" s="10">
-        <v>1110100</v>
+        <v>1110010</v>
       </c>
       <c r="E57" s="3" t="str">
-        <f t="shared" ref="E57:E58" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C57,7) + BIN2DEC($D57)))</f>
-        <v>0x74</v>
+        <f t="shared" si="1"/>
+        <v>0x72</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>17</v>
@@ -6190,7 +6211,7 @@
         <v>105</v>
       </c>
       <c r="Z57" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AA57" s="23" t="s">
         <v>145</v>
@@ -6199,12 +6220,12 @@
         <v>100</v>
       </c>
       <c r="AC57" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>72</v>
@@ -6213,82 +6234,262 @@
         <v>0</v>
       </c>
       <c r="D58" s="10">
+        <v>1110011</v>
+      </c>
+      <c r="E58" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x73</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L58" s="6">
+        <v>0</v>
+      </c>
+      <c r="M58" s="6">
+        <v>0</v>
+      </c>
+      <c r="N58" s="6">
+        <v>0</v>
+      </c>
+      <c r="O58" s="6">
+        <v>0</v>
+      </c>
+      <c r="P58" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>0</v>
+      </c>
+      <c r="R58" s="6">
+        <v>0</v>
+      </c>
+      <c r="S58" s="6">
+        <v>0</v>
+      </c>
+      <c r="T58" s="6">
+        <v>0</v>
+      </c>
+      <c r="U58" s="6">
+        <v>1</v>
+      </c>
+      <c r="V58" s="6">
+        <v>1</v>
+      </c>
+      <c r="W58" s="6">
+        <v>0</v>
+      </c>
+      <c r="X58" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y58" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z58" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA58" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0</v>
+      </c>
+      <c r="D59" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E59" s="3" t="str">
+        <f t="shared" ref="E59:E60" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C59,7) + BIN2DEC($D59)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K59" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L59" s="6">
+        <v>0</v>
+      </c>
+      <c r="M59" s="6">
+        <v>0</v>
+      </c>
+      <c r="N59" s="6">
+        <v>0</v>
+      </c>
+      <c r="O59" s="6">
+        <v>0</v>
+      </c>
+      <c r="P59" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="6">
+        <v>0</v>
+      </c>
+      <c r="R59" s="6">
+        <v>0</v>
+      </c>
+      <c r="S59" s="6">
+        <v>0</v>
+      </c>
+      <c r="T59" s="6">
+        <v>0</v>
+      </c>
+      <c r="U59" s="6">
+        <v>1</v>
+      </c>
+      <c r="V59" s="6">
+        <v>1</v>
+      </c>
+      <c r="W59" s="6">
+        <v>0</v>
+      </c>
+      <c r="X59" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y59" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z59" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA59" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0</v>
+      </c>
+      <c r="D60" s="10">
         <v>1111000</v>
       </c>
-      <c r="E58" s="3" t="str">
+      <c r="E60" s="3" t="str">
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G58" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L58" s="6">
-        <v>0</v>
-      </c>
-      <c r="M58" s="6">
-        <v>0</v>
-      </c>
-      <c r="N58" s="6">
-        <v>0</v>
-      </c>
-      <c r="O58" s="6">
-        <v>0</v>
-      </c>
-      <c r="P58" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="6">
-        <v>0</v>
-      </c>
-      <c r="R58" s="6">
-        <v>0</v>
-      </c>
-      <c r="S58" s="6">
-        <v>0</v>
-      </c>
-      <c r="T58" s="6">
-        <v>0</v>
-      </c>
-      <c r="U58" s="6">
-        <v>1</v>
-      </c>
-      <c r="V58" s="6">
-        <v>1</v>
-      </c>
-      <c r="W58" s="6">
-        <v>0</v>
-      </c>
-      <c r="X58" s="13" t="s">
+      <c r="F60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L60" s="6">
+        <v>0</v>
+      </c>
+      <c r="M60" s="6">
+        <v>0</v>
+      </c>
+      <c r="N60" s="6">
+        <v>0</v>
+      </c>
+      <c r="O60" s="6">
+        <v>0</v>
+      </c>
+      <c r="P60" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="6">
+        <v>0</v>
+      </c>
+      <c r="R60" s="6">
+        <v>0</v>
+      </c>
+      <c r="S60" s="6">
+        <v>0</v>
+      </c>
+      <c r="T60" s="6">
+        <v>0</v>
+      </c>
+      <c r="U60" s="6">
+        <v>1</v>
+      </c>
+      <c r="V60" s="6">
+        <v>1</v>
+      </c>
+      <c r="W60" s="6">
+        <v>0</v>
+      </c>
+      <c r="X60" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y58" s="22" t="s">
+      <c r="Y60" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="Z58" s="3" t="s">
+      <c r="Z60" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AA58" s="23" t="s">
+      <c r="AA60" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="AB58" t="s">
+      <c r="AB60" t="s">
         <v>100</v>
       </c>
-      <c r="AC58" t="s">
+      <c r="AC60" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding buffer read macor
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10476DA1-D5DB-5245-889F-B5D69DA9DF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB69FF31-007D-864D-8957-8C3449A5A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="215">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>read CMOS QL size</t>
+  </si>
+  <si>
+    <t>read_ql_data</t>
   </si>
 </sst>
 </file>
@@ -1175,13 +1178,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC60"/>
+  <dimension ref="A1:AC61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC28" sqref="AC28"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E31" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E32" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -3857,7 +3860,7 @@
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>72</v>
@@ -3866,11 +3869,11 @@
         <v>1</v>
       </c>
       <c r="D31" s="10">
-        <v>10101</v>
+        <v>11111</v>
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x95</v>
+        <v>0x9F</v>
       </c>
       <c r="F31" s="27" t="s">
         <v>17</v>
@@ -3884,11 +3887,11 @@
       <c r="I31" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="J31" s="33" t="s">
-        <v>201</v>
+      <c r="J31" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>206</v>
+        <v>102</v>
       </c>
       <c r="L31" s="30">
         <v>0</v>
@@ -3932,8 +3935,8 @@
       <c r="Y31" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="Z31" s="27" t="s">
-        <v>205</v>
+      <c r="Z31" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="AA31" s="25" t="s">
         <v>57</v>
@@ -3945,127 +3948,127 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="24"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="24"/>
+    <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="27">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10">
+        <v>10101</v>
+      </c>
+      <c r="E32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0x95</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L32" s="30">
+        <v>0</v>
+      </c>
+      <c r="M32" s="30">
+        <v>0</v>
+      </c>
+      <c r="N32" s="30">
+        <v>0</v>
+      </c>
+      <c r="O32" s="30">
+        <v>0</v>
+      </c>
+      <c r="P32" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="30">
+        <v>0</v>
+      </c>
+      <c r="R32" s="30">
+        <v>0</v>
+      </c>
+      <c r="S32" s="30">
+        <v>0</v>
+      </c>
+      <c r="T32" s="30">
+        <v>0</v>
+      </c>
+      <c r="U32" s="30">
+        <v>1</v>
+      </c>
+      <c r="V32" s="30">
+        <v>1</v>
+      </c>
+      <c r="W32" s="31">
+        <v>0</v>
+      </c>
+      <c r="X32" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y32" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z32" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA32" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB32" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC32" s="28" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="10">
-        <v>1000000</v>
-      </c>
-      <c r="E33" s="3" t="str">
-        <f t="shared" ref="E33:E58" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C33,7) + BIN2DEC($D33)))</f>
-        <v>0x40</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K33" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L33" s="6">
-        <v>0</v>
-      </c>
-      <c r="M33" s="6">
-        <v>1</v>
-      </c>
-      <c r="N33" s="6">
-        <v>0</v>
-      </c>
-      <c r="O33" s="6">
-        <v>0</v>
-      </c>
-      <c r="P33" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="6">
-        <v>0</v>
-      </c>
-      <c r="R33" s="6">
-        <v>0</v>
-      </c>
-      <c r="S33" s="6">
-        <v>0</v>
-      </c>
-      <c r="T33" s="6">
-        <v>0</v>
-      </c>
-      <c r="U33" s="6">
-        <v>0</v>
-      </c>
-      <c r="V33" s="6">
-        <v>0</v>
-      </c>
-      <c r="W33" s="16">
-        <v>0</v>
-      </c>
-      <c r="X33" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y33" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z33" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA33" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>77</v>
-      </c>
+    <row r="33" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="24"/>
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>72</v>
@@ -4074,11 +4077,11 @@
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>1000010</v>
+        <v>1000000</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x42</v>
+        <f t="shared" ref="E34:E59" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C34,7) + BIN2DEC($D34)))</f>
+        <v>0x40</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>53</v>
@@ -4150,12 +4153,12 @@
         <v>100</v>
       </c>
       <c r="AC34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>72</v>
@@ -4164,17 +4167,17 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>1000100</v>
+        <v>1000010</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x44</v>
+        <v>0x42</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>17</v>
@@ -4189,10 +4192,10 @@
         <v>57</v>
       </c>
       <c r="L35" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="6">
         <v>0</v>
@@ -4240,12 +4243,12 @@
         <v>100</v>
       </c>
       <c r="AC35" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>72</v>
@@ -4254,11 +4257,11 @@
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>1000101</v>
+        <v>1000100</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x45</v>
+        <v>0x44</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>17</v>
@@ -4335,7 +4338,7 @@
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>72</v>
@@ -4344,17 +4347,17 @@
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>1110111</v>
+        <v>1000101</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0x45</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>17</v>
@@ -4420,12 +4423,12 @@
         <v>100</v>
       </c>
       <c r="AC37" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>72</v>
@@ -4434,14 +4437,14 @@
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>1100001</v>
+        <v>1110111</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x77</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G38">
         <v>2</v>
@@ -4459,7 +4462,7 @@
         <v>57</v>
       </c>
       <c r="L38" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="6">
         <v>0</v>
@@ -4471,19 +4474,19 @@
         <v>0</v>
       </c>
       <c r="P38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U38" s="6">
         <v>0</v>
@@ -4492,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="W38" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X38" s="13" t="s">
         <v>97</v>
@@ -4510,12 +4513,12 @@
         <v>100</v>
       </c>
       <c r="AC38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>72</v>
@@ -4524,17 +4527,17 @@
         <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>1100010</v>
+        <v>1100001</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x61</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>17</v>
@@ -4600,12 +4603,12 @@
         <v>100</v>
       </c>
       <c r="AC39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>72</v>
@@ -4614,11 +4617,11 @@
         <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>1100011</v>
+        <v>1100010</v>
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x62</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>17</v>
@@ -4690,12 +4693,12 @@
         <v>100</v>
       </c>
       <c r="AC40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>72</v>
@@ -4704,11 +4707,11 @@
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>100100</v>
+        <v>1100011</v>
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x24</v>
+        <v>0x63</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -4729,10 +4732,10 @@
         <v>57</v>
       </c>
       <c r="L41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" s="6">
         <v>0</v>
@@ -4756,10 +4759,10 @@
         <v>1</v>
       </c>
       <c r="U41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W41" s="16">
         <v>1</v>
@@ -4780,12 +4783,12 @@
         <v>100</v>
       </c>
       <c r="AC41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>72</v>
@@ -4794,11 +4797,11 @@
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>100101</v>
+        <v>100100</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x25</v>
+        <v>0x24</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>17</v>
@@ -4870,12 +4873,12 @@
         <v>100</v>
       </c>
       <c r="AC42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
-        <v>107</v>
+    <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>72</v>
@@ -4884,11 +4887,11 @@
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>11000</v>
+        <v>100101</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C43,7) + BIN2DEC($D43)))</f>
-        <v>0x18</v>
+        <f t="shared" si="1"/>
+        <v>0x25</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>17</v>
@@ -4909,10 +4912,10 @@
         <v>57</v>
       </c>
       <c r="L43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N43" s="6">
         <v>0</v>
@@ -4921,19 +4924,19 @@
         <v>0</v>
       </c>
       <c r="P43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U43" s="6">
         <v>1</v>
@@ -4942,7 +4945,7 @@
         <v>1</v>
       </c>
       <c r="W43" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X43" s="13" t="s">
         <v>97</v>
@@ -4951,21 +4954,21 @@
         <v>105</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA43" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA43" s="23">
+        <v>0</v>
       </c>
       <c r="AB43" t="s">
         <v>100</v>
       </c>
       <c r="AC43" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>72</v>
@@ -4974,11 +4977,11 @@
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>11111</v>
+        <v>11000</v>
       </c>
       <c r="E44" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1F</v>
+        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C44,7) + BIN2DEC($D44)))</f>
+        <v>0x18</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>17</v>
@@ -4992,7 +4995,7 @@
       <c r="I44" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K44" s="23" t="s">
@@ -5041,7 +5044,7 @@
         <v>105</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AA44" s="23" t="s">
         <v>145</v>
@@ -5050,12 +5053,12 @@
         <v>100</v>
       </c>
       <c r="AC44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>72</v>
@@ -5064,11 +5067,11 @@
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>10000</v>
+        <v>11111</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x10</v>
+        <v>0x1F</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>17</v>
@@ -5131,7 +5134,7 @@
         <v>105</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA45" s="23" t="s">
         <v>145</v>
@@ -5140,12 +5143,12 @@
         <v>100</v>
       </c>
       <c r="AC45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>106</v>
+      <c r="A46" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>72</v>
@@ -5154,11 +5157,11 @@
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>10001</v>
+        <v>10000</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x11</v>
+        <v>0x10</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>17</v>
@@ -5221,21 +5224,21 @@
         <v>105</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="AA46" s="23" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="AB46" t="s">
         <v>100</v>
       </c>
       <c r="AC46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
-        <v>117</v>
+      <c r="A47" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>72</v>
@@ -5244,11 +5247,11 @@
         <v>0</v>
       </c>
       <c r="D47" s="10">
-        <v>10010</v>
+        <v>10001</v>
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x12</v>
+        <v>0x11</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>17</v>
@@ -5311,21 +5314,21 @@
         <v>105</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="AA47" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="AB47" t="s">
         <v>100</v>
       </c>
       <c r="AC47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>72</v>
@@ -5334,11 +5337,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="10">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x13</v>
+        <v>0x12</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>17</v>
@@ -5401,7 +5404,7 @@
         <v>105</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AA48" s="23" t="s">
         <v>145</v>
@@ -5410,12 +5413,12 @@
         <v>100</v>
       </c>
       <c r="AC48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>50</v>
+      <c r="A49" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>72</v>
@@ -5424,17 +5427,17 @@
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>11010</v>
+        <v>10011</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1A</v>
+        <v>0x13</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>17</v>
@@ -5442,7 +5445,7 @@
       <c r="I49" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J49" s="3" t="s">
+      <c r="J49" t="s">
         <v>17</v>
       </c>
       <c r="K49" s="23" t="s">
@@ -5461,25 +5464,25 @@
         <v>0</v>
       </c>
       <c r="P49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T49" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49" s="16">
         <v>0</v>
@@ -5491,21 +5494,21 @@
         <v>105</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA49" s="23">
-        <v>0</v>
+        <v>123</v>
+      </c>
+      <c r="AA49" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="AB49" t="s">
         <v>100</v>
       </c>
       <c r="AC49" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>72</v>
@@ -5514,17 +5517,17 @@
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <v>11100</v>
+        <v>11010</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1C</v>
+        <v>0x1A</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G50" t="s">
-        <v>97</v>
+        <v>51</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>17</v>
@@ -5590,12 +5593,12 @@
         <v>100</v>
       </c>
       <c r="AC50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>72</v>
@@ -5604,14 +5607,14 @@
         <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>11101</v>
+        <v>11100</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1D</v>
+        <v>0x1C</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="G51" t="s">
         <v>97</v>
@@ -5680,12 +5683,12 @@
         <v>100</v>
       </c>
       <c r="AC51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>72</v>
@@ -5694,14 +5697,14 @@
         <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>111010</v>
+        <v>11101</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3A</v>
+        <v>0x1D</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="G52" t="s">
         <v>97</v>
@@ -5731,25 +5734,25 @@
         <v>0</v>
       </c>
       <c r="P52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T52" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U52" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V52" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W52" s="16">
         <v>0</v>
@@ -5770,12 +5773,12 @@
         <v>100</v>
       </c>
       <c r="AC52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>72</v>
@@ -5784,11 +5787,11 @@
         <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>111011</v>
+        <v>111010</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3B</v>
+        <v>0x3A</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>99</v>
@@ -5860,12 +5863,12 @@
         <v>100</v>
       </c>
       <c r="AC53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>72</v>
@@ -5874,17 +5877,17 @@
         <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>111001</v>
+        <v>111011</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x39</v>
+        <v>0x3B</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="G54" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>17</v>
@@ -5899,7 +5902,7 @@
         <v>57</v>
       </c>
       <c r="L54" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54" s="6">
         <v>0</v>
@@ -5926,10 +5929,10 @@
         <v>0</v>
       </c>
       <c r="U54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W54" s="16">
         <v>0</v>
@@ -5950,12 +5953,12 @@
         <v>100</v>
       </c>
       <c r="AC54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
-        <v>36</v>
+      <c r="A55" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>72</v>
@@ -5964,11 +5967,11 @@
         <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>1110000</v>
+        <v>111001</v>
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x39</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>17</v>
@@ -5989,7 +5992,7 @@
         <v>57</v>
       </c>
       <c r="L55" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M55" s="6">
         <v>0</v>
@@ -6016,12 +6019,12 @@
         <v>0</v>
       </c>
       <c r="U55" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V55" s="6">
-        <v>1</v>
-      </c>
-      <c r="W55" s="6">
+        <v>0</v>
+      </c>
+      <c r="W55" s="16">
         <v>0</v>
       </c>
       <c r="X55" s="13" t="s">
@@ -6031,21 +6034,21 @@
         <v>105</v>
       </c>
       <c r="Z55" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA55" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA55" s="23">
+        <v>0</v>
       </c>
       <c r="AB55" t="s">
         <v>100</v>
       </c>
       <c r="AC55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>72</v>
@@ -6054,11 +6057,11 @@
         <v>0</v>
       </c>
       <c r="D56" s="10">
-        <v>1110001</v>
+        <v>1110000</v>
       </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x70</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>17</v>
@@ -6121,7 +6124,7 @@
         <v>105</v>
       </c>
       <c r="Z56" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AA56" s="23" t="s">
         <v>145</v>
@@ -6130,12 +6133,12 @@
         <v>100</v>
       </c>
       <c r="AC56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>72</v>
@@ -6144,11 +6147,11 @@
         <v>0</v>
       </c>
       <c r="D57" s="10">
-        <v>1110010</v>
+        <v>1110001</v>
       </c>
       <c r="E57" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x71</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>17</v>
@@ -6211,7 +6214,7 @@
         <v>105</v>
       </c>
       <c r="Z57" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA57" s="23" t="s">
         <v>145</v>
@@ -6220,12 +6223,12 @@
         <v>100</v>
       </c>
       <c r="AC57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>72</v>
@@ -6234,11 +6237,11 @@
         <v>0</v>
       </c>
       <c r="D58" s="10">
-        <v>1110011</v>
+        <v>1110010</v>
       </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x72</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>17</v>
@@ -6301,7 +6304,7 @@
         <v>105</v>
       </c>
       <c r="Z58" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AA58" s="23" t="s">
         <v>145</v>
@@ -6310,12 +6313,12 @@
         <v>100</v>
       </c>
       <c r="AC58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>72</v>
@@ -6324,11 +6327,11 @@
         <v>0</v>
       </c>
       <c r="D59" s="10">
-        <v>1110100</v>
+        <v>1110011</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f t="shared" ref="E59:E60" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C59,7) + BIN2DEC($D59)))</f>
-        <v>0x74</v>
+        <f t="shared" si="1"/>
+        <v>0x73</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>17</v>
@@ -6391,7 +6394,7 @@
         <v>105</v>
       </c>
       <c r="Z59" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AA59" s="23" t="s">
         <v>145</v>
@@ -6400,12 +6403,12 @@
         <v>100</v>
       </c>
       <c r="AC59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>72</v>
@@ -6414,82 +6417,172 @@
         <v>0</v>
       </c>
       <c r="D60" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E60" s="3" t="str">
+        <f t="shared" ref="E60:E61" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C60,7) + BIN2DEC($D60)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L60" s="6">
+        <v>0</v>
+      </c>
+      <c r="M60" s="6">
+        <v>0</v>
+      </c>
+      <c r="N60" s="6">
+        <v>0</v>
+      </c>
+      <c r="O60" s="6">
+        <v>0</v>
+      </c>
+      <c r="P60" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="6">
+        <v>0</v>
+      </c>
+      <c r="R60" s="6">
+        <v>0</v>
+      </c>
+      <c r="S60" s="6">
+        <v>0</v>
+      </c>
+      <c r="T60" s="6">
+        <v>0</v>
+      </c>
+      <c r="U60" s="6">
+        <v>1</v>
+      </c>
+      <c r="V60" s="6">
+        <v>1</v>
+      </c>
+      <c r="W60" s="6">
+        <v>0</v>
+      </c>
+      <c r="X60" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y60" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z60" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA60" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0</v>
+      </c>
+      <c r="D61" s="10">
         <v>1111000</v>
       </c>
-      <c r="E60" s="3" t="str">
+      <c r="E61" s="3" t="str">
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G60" t="s">
-        <v>17</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I60" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K60" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L60" s="6">
-        <v>0</v>
-      </c>
-      <c r="M60" s="6">
-        <v>0</v>
-      </c>
-      <c r="N60" s="6">
-        <v>0</v>
-      </c>
-      <c r="O60" s="6">
-        <v>0</v>
-      </c>
-      <c r="P60" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="6">
-        <v>0</v>
-      </c>
-      <c r="R60" s="6">
-        <v>0</v>
-      </c>
-      <c r="S60" s="6">
-        <v>0</v>
-      </c>
-      <c r="T60" s="6">
-        <v>0</v>
-      </c>
-      <c r="U60" s="6">
-        <v>1</v>
-      </c>
-      <c r="V60" s="6">
-        <v>1</v>
-      </c>
-      <c r="W60" s="6">
-        <v>0</v>
-      </c>
-      <c r="X60" s="13" t="s">
+      <c r="F61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L61" s="6">
+        <v>0</v>
+      </c>
+      <c r="M61" s="6">
+        <v>0</v>
+      </c>
+      <c r="N61" s="6">
+        <v>0</v>
+      </c>
+      <c r="O61" s="6">
+        <v>0</v>
+      </c>
+      <c r="P61" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="6">
+        <v>0</v>
+      </c>
+      <c r="R61" s="6">
+        <v>0</v>
+      </c>
+      <c r="S61" s="6">
+        <v>0</v>
+      </c>
+      <c r="T61" s="6">
+        <v>0</v>
+      </c>
+      <c r="U61" s="6">
+        <v>1</v>
+      </c>
+      <c r="V61" s="6">
+        <v>1</v>
+      </c>
+      <c r="W61" s="6">
+        <v>0</v>
+      </c>
+      <c r="X61" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y60" s="22" t="s">
+      <c r="Y61" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="Z60" s="3" t="s">
+      <c r="Z61" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AA60" s="23" t="s">
+      <c r="AA61" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="AB60" t="s">
+      <c r="AB61" t="s">
         <v>100</v>
       </c>
-      <c r="AC60" t="s">
+      <c r="AC61" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding double command enable for cmos shutdown
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB69FF31-007D-864D-8957-8C3449A5A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13695E72-0290-E64C-BD6F-9A17122634A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="219">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -679,6 +679,18 @@
   </si>
   <si>
     <t>read_ql_data</t>
+  </si>
+  <si>
+    <t>enable_double_cmds</t>
+  </si>
+  <si>
+    <t>shutdown_cmos</t>
+  </si>
+  <si>
+    <t>0x0000018c</t>
+  </si>
+  <si>
+    <t>0x00000180</t>
   </si>
 </sst>
 </file>
@@ -1178,13 +1190,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC61"/>
+  <dimension ref="A1:AC63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="AA51" sqref="AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -4080,7 +4092,7 @@
         <v>1000000</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f t="shared" ref="E34:E59" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C34,7) + BIN2DEC($D34)))</f>
+        <f t="shared" ref="E34:E61" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C34,7) + BIN2DEC($D34)))</f>
         <v>0x40</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -5507,8 +5519,8 @@
       </c>
     </row>
     <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>50</v>
+      <c r="A50" s="19" t="s">
+        <v>215</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>72</v>
@@ -5517,17 +5529,17 @@
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <v>11010</v>
+        <v>1111</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1A</v>
+        <v>0xF</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>17</v>
@@ -5535,7 +5547,7 @@
       <c r="I50" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J50" s="3" t="s">
+      <c r="J50" t="s">
         <v>17</v>
       </c>
       <c r="K50" s="23" t="s">
@@ -5554,25 +5566,25 @@
         <v>0</v>
       </c>
       <c r="P50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="16">
         <v>0</v>
@@ -5584,21 +5596,21 @@
         <v>105</v>
       </c>
       <c r="Z50" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA50" s="23">
-        <v>0</v>
+        <v>218</v>
+      </c>
+      <c r="AA50" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="AB50" t="s">
         <v>100</v>
       </c>
       <c r="AC50" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>47</v>
+      <c r="A51" s="19" t="s">
+        <v>216</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>72</v>
@@ -5607,17 +5619,17 @@
         <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>11100</v>
+        <v>1100</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1C</v>
+        <v>0xC</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="G51" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>17</v>
@@ -5625,7 +5637,7 @@
       <c r="I51" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="J51" t="s">
         <v>17</v>
       </c>
       <c r="K51" s="23" t="s">
@@ -5644,25 +5656,25 @@
         <v>0</v>
       </c>
       <c r="P51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W51" s="16">
         <v>0</v>
@@ -5674,21 +5686,21 @@
         <v>105</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA51" s="23">
-        <v>0</v>
+        <v>217</v>
+      </c>
+      <c r="AA51" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="AB51" t="s">
         <v>100</v>
       </c>
       <c r="AC51" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>72</v>
@@ -5697,17 +5709,17 @@
         <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>11101</v>
+        <v>11010</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1D</v>
+        <v>0x1A</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G52" t="s">
-        <v>97</v>
+        <v>51</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>17</v>
@@ -5773,12 +5785,12 @@
         <v>100</v>
       </c>
       <c r="AC52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>72</v>
@@ -5787,14 +5799,14 @@
         <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>111010</v>
+        <v>11100</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3A</v>
+        <v>0x1C</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G53" t="s">
         <v>97</v>
@@ -5824,25 +5836,25 @@
         <v>0</v>
       </c>
       <c r="P53" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q53" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R53" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S53" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V53" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W53" s="16">
         <v>0</v>
@@ -5863,12 +5875,12 @@
         <v>100</v>
       </c>
       <c r="AC53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>72</v>
@@ -5877,14 +5889,14 @@
         <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>111011</v>
+        <v>11101</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3B</v>
+        <v>0x1D</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="G54" t="s">
         <v>97</v>
@@ -5914,25 +5926,25 @@
         <v>0</v>
       </c>
       <c r="P54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U54" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V54" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W54" s="16">
         <v>0</v>
@@ -5953,12 +5965,12 @@
         <v>100</v>
       </c>
       <c r="AC54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>72</v>
@@ -5967,17 +5979,17 @@
         <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>111001</v>
+        <v>111010</v>
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x39</v>
+        <v>0x3A</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="G55" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>17</v>
@@ -5992,7 +6004,7 @@
         <v>57</v>
       </c>
       <c r="L55" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55" s="6">
         <v>0</v>
@@ -6019,10 +6031,10 @@
         <v>0</v>
       </c>
       <c r="U55" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W55" s="16">
         <v>0</v>
@@ -6043,12 +6055,12 @@
         <v>100</v>
       </c>
       <c r="AC55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="19" t="s">
-        <v>36</v>
+      <c r="A56" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>72</v>
@@ -6057,17 +6069,17 @@
         <v>0</v>
       </c>
       <c r="D56" s="10">
-        <v>1110000</v>
+        <v>111011</v>
       </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x3B</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="G56" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>17</v>
@@ -6114,7 +6126,7 @@
       <c r="V56" s="6">
         <v>1</v>
       </c>
-      <c r="W56" s="6">
+      <c r="W56" s="16">
         <v>0</v>
       </c>
       <c r="X56" s="13" t="s">
@@ -6124,21 +6136,21 @@
         <v>105</v>
       </c>
       <c r="Z56" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA56" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA56" s="23">
+        <v>0</v>
       </c>
       <c r="AB56" t="s">
         <v>100</v>
       </c>
       <c r="AC56" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
-        <v>37</v>
+      <c r="A57" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>72</v>
@@ -6147,11 +6159,11 @@
         <v>0</v>
       </c>
       <c r="D57" s="10">
-        <v>1110001</v>
+        <v>111001</v>
       </c>
       <c r="E57" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x39</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>17</v>
@@ -6172,7 +6184,7 @@
         <v>57</v>
       </c>
       <c r="L57" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M57" s="6">
         <v>0</v>
@@ -6199,12 +6211,12 @@
         <v>0</v>
       </c>
       <c r="U57" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V57" s="6">
-        <v>1</v>
-      </c>
-      <c r="W57" s="6">
+        <v>0</v>
+      </c>
+      <c r="W57" s="16">
         <v>0</v>
       </c>
       <c r="X57" s="13" t="s">
@@ -6214,21 +6226,21 @@
         <v>105</v>
       </c>
       <c r="Z57" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA57" s="23" t="s">
-        <v>145</v>
+        <v>57</v>
+      </c>
+      <c r="AA57" s="23">
+        <v>0</v>
       </c>
       <c r="AB57" t="s">
         <v>100</v>
       </c>
       <c r="AC57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>72</v>
@@ -6237,11 +6249,11 @@
         <v>0</v>
       </c>
       <c r="D58" s="10">
-        <v>1110010</v>
+        <v>1110000</v>
       </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x70</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>17</v>
@@ -6304,7 +6316,7 @@
         <v>105</v>
       </c>
       <c r="Z58" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AA58" s="23" t="s">
         <v>145</v>
@@ -6313,12 +6325,12 @@
         <v>100</v>
       </c>
       <c r="AC58" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>72</v>
@@ -6327,11 +6339,11 @@
         <v>0</v>
       </c>
       <c r="D59" s="10">
-        <v>1110011</v>
+        <v>1110001</v>
       </c>
       <c r="E59" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x71</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>17</v>
@@ -6394,7 +6406,7 @@
         <v>105</v>
       </c>
       <c r="Z59" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AA59" s="23" t="s">
         <v>145</v>
@@ -6403,12 +6415,12 @@
         <v>100</v>
       </c>
       <c r="AC59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>72</v>
@@ -6417,11 +6429,11 @@
         <v>0</v>
       </c>
       <c r="D60" s="10">
-        <v>1110100</v>
+        <v>1110010</v>
       </c>
       <c r="E60" s="3" t="str">
-        <f t="shared" ref="E60:E61" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C60,7) + BIN2DEC($D60)))</f>
-        <v>0x74</v>
+        <f t="shared" si="1"/>
+        <v>0x72</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>17</v>
@@ -6484,7 +6496,7 @@
         <v>105</v>
       </c>
       <c r="Z60" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AA60" s="23" t="s">
         <v>145</v>
@@ -6493,12 +6505,12 @@
         <v>100</v>
       </c>
       <c r="AC60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>72</v>
@@ -6507,82 +6519,262 @@
         <v>0</v>
       </c>
       <c r="D61" s="10">
+        <v>1110011</v>
+      </c>
+      <c r="E61" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x73</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L61" s="6">
+        <v>0</v>
+      </c>
+      <c r="M61" s="6">
+        <v>0</v>
+      </c>
+      <c r="N61" s="6">
+        <v>0</v>
+      </c>
+      <c r="O61" s="6">
+        <v>0</v>
+      </c>
+      <c r="P61" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="6">
+        <v>0</v>
+      </c>
+      <c r="R61" s="6">
+        <v>0</v>
+      </c>
+      <c r="S61" s="6">
+        <v>0</v>
+      </c>
+      <c r="T61" s="6">
+        <v>0</v>
+      </c>
+      <c r="U61" s="6">
+        <v>1</v>
+      </c>
+      <c r="V61" s="6">
+        <v>1</v>
+      </c>
+      <c r="W61" s="6">
+        <v>0</v>
+      </c>
+      <c r="X61" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y61" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z61" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA61" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0</v>
+      </c>
+      <c r="D62" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E62" s="3" t="str">
+        <f t="shared" ref="E62:E63" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C62,7) + BIN2DEC($D62)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K62" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L62" s="6">
+        <v>0</v>
+      </c>
+      <c r="M62" s="6">
+        <v>0</v>
+      </c>
+      <c r="N62" s="6">
+        <v>0</v>
+      </c>
+      <c r="O62" s="6">
+        <v>0</v>
+      </c>
+      <c r="P62" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="6">
+        <v>0</v>
+      </c>
+      <c r="R62" s="6">
+        <v>0</v>
+      </c>
+      <c r="S62" s="6">
+        <v>0</v>
+      </c>
+      <c r="T62" s="6">
+        <v>0</v>
+      </c>
+      <c r="U62" s="6">
+        <v>1</v>
+      </c>
+      <c r="V62" s="6">
+        <v>1</v>
+      </c>
+      <c r="W62" s="6">
+        <v>0</v>
+      </c>
+      <c r="X62" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y62" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z62" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA62" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0</v>
+      </c>
+      <c r="D63" s="10">
         <v>1111000</v>
       </c>
-      <c r="E61" s="3" t="str">
+      <c r="E63" s="3" t="str">
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G61" t="s">
-        <v>17</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I61" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K61" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L61" s="6">
-        <v>0</v>
-      </c>
-      <c r="M61" s="6">
-        <v>0</v>
-      </c>
-      <c r="N61" s="6">
-        <v>0</v>
-      </c>
-      <c r="O61" s="6">
-        <v>0</v>
-      </c>
-      <c r="P61" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="6">
-        <v>0</v>
-      </c>
-      <c r="R61" s="6">
-        <v>0</v>
-      </c>
-      <c r="S61" s="6">
-        <v>0</v>
-      </c>
-      <c r="T61" s="6">
-        <v>0</v>
-      </c>
-      <c r="U61" s="6">
-        <v>1</v>
-      </c>
-      <c r="V61" s="6">
-        <v>1</v>
-      </c>
-      <c r="W61" s="6">
-        <v>0</v>
-      </c>
-      <c r="X61" s="13" t="s">
+      <c r="F63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K63" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L63" s="6">
+        <v>0</v>
+      </c>
+      <c r="M63" s="6">
+        <v>0</v>
+      </c>
+      <c r="N63" s="6">
+        <v>0</v>
+      </c>
+      <c r="O63" s="6">
+        <v>0</v>
+      </c>
+      <c r="P63" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="6">
+        <v>0</v>
+      </c>
+      <c r="R63" s="6">
+        <v>0</v>
+      </c>
+      <c r="S63" s="6">
+        <v>0</v>
+      </c>
+      <c r="T63" s="6">
+        <v>0</v>
+      </c>
+      <c r="U63" s="6">
+        <v>1</v>
+      </c>
+      <c r="V63" s="6">
+        <v>1</v>
+      </c>
+      <c r="W63" s="6">
+        <v>0</v>
+      </c>
+      <c r="X63" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y61" s="22" t="s">
+      <c r="Y63" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="Z61" s="3" t="s">
+      <c r="Z63" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AA61" s="23" t="s">
+      <c r="AA63" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="AB61" t="s">
+      <c r="AB63" t="s">
         <v>100</v>
       </c>
-      <c r="AC61" t="s">
+      <c r="AC63" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correcting shutdown and doublecommand memory address for cmos
</commit_message>
<xml_diff>
--- a/cmos_command_deck.xlsx
+++ b/cmos_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13695E72-0290-E64C-BD6F-9A17122634A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0662C359-76DF-9F47-8029-AE1EAFDB0FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -687,10 +687,10 @@
     <t>shutdown_cmos</t>
   </si>
   <si>
-    <t>0x0000018c</t>
-  </si>
-  <si>
-    <t>0x00000180</t>
+    <t>0x00000080</t>
+  </si>
+  <si>
+    <t>0x0000008c</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1193,10 @@
   <dimension ref="A1:AC63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="N25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA51" sqref="AA51"/>
+      <selection pane="bottomRight" activeCell="Z51" sqref="Z51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -5596,7 +5596,7 @@
         <v>105</v>
       </c>
       <c r="Z50" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AA50" s="23" t="s">
         <v>145</v>
@@ -5686,7 +5686,7 @@
         <v>105</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AA51" s="23" t="s">
         <v>145</v>

</xml_diff>